<commit_message>
Excel package. Format copy implementation.
</commit_message>
<xml_diff>
--- a/examples/excel/sheets-copying/src/main/resources/sample.xlsx
+++ b/examples/excel/sheets-copying/src/main/resources/sample.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EasyRPA\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\-=PROJECTS=-\EasyRPA\Work\easy-rpa-openframework\examples\excel\sheets-copying\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet with Image" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>

</xml_diff>